<commit_message>
Assure that files uploaded through web forms and files generated from templates can be cross-referenced to known document requirements from the protocol builder.  Configurators can control this by managing an XLS Spreadsheet called "irb_documents.xslx". Required Documents is becoming complicated, so making this it's own script task, removing it from study_info.py The file_service is now very aware of this irb_documents file, so it will always need to exist.  We seed this file during setup, but it can be overwritten by the configurator.
</commit_message>
<xml_diff>
--- a/tests/data/reference/irb_documents.xlsx
+++ b/tests/data/reference/irb_documents.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="234">
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
   <si>
     <t xml:space="preserve">category1</t>
   </si>
@@ -40,6 +43,9 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">AncillaryDocument.CoCApplication</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ancillary Document</t>
   </si>
   <si>
@@ -55,171 +61,306 @@
     <t xml:space="preserve">Certificate of Confidentiality Application</t>
   </si>
   <si>
+    <t xml:space="preserve">AncillaryDocument.Consent.Model</t>
+  </si>
+  <si>
     <t xml:space="preserve">Consent</t>
   </si>
   <si>
     <t xml:space="preserve">Model</t>
   </si>
   <si>
+    <t xml:space="preserve">AncillaryDocument.Consent.StandardRadiationConsentLanguage</t>
+  </si>
+  <si>
     <t xml:space="preserve">Standard Radiation Consent Language</t>
   </si>
   <si>
     <t xml:space="preserve">HIRE Standard Radiation Language</t>
   </si>
   <si>
+    <t xml:space="preserve">AncillaryDocument.IRBApprovalNon-UVAForeign</t>
+  </si>
+  <si>
     <t xml:space="preserve">IRB Approval Non-UVA Foreign</t>
   </si>
   <si>
+    <t xml:space="preserve">AncillaryDocument.IRBApprovalNon-UVAUSA</t>
+  </si>
+  <si>
     <t xml:space="preserve">IRB Approval Non-UVA USA</t>
   </si>
   <si>
+    <t xml:space="preserve">AncillaryDocument.LabManual</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lab Manual</t>
   </si>
   <si>
+    <t xml:space="preserve">AncillaryDocument.ManualofOperations</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manual of Operations</t>
   </si>
   <si>
+    <t xml:space="preserve">AncillaryDocument.Non-UVAInstitutionalApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non-UVA Institutional Approval</t>
   </si>
   <si>
+    <t xml:space="preserve">AncillaryDocument.ReminderCard</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reminder Card</t>
   </si>
   <si>
+    <t xml:space="preserve">AncillaryDocument.SubjectDiary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Subject Diary</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.Addendum.Other</t>
+  </si>
+  <si>
     <t xml:space="preserve">Addendum</t>
   </si>
   <si>
     <t xml:space="preserve">Other</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.Addendum.PregnantPartner</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pregnant Partner</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.Adult</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adult</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.AdultParentalPermission</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adult Parental Permission</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.AdultParentalPermissionMinorAssent</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adult Parental Permission Minor Assent</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.AgeofMajority</t>
+  </si>
+  <si>
     <t xml:space="preserve">Age of Majority</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.AgeofMajorityCoverLetter</t>
+  </si>
+  <si>
     <t xml:space="preserve">Age of Majority Cover Letter</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.AssentForm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assent Form</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.DryRun</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dry Run</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.ParentalPermission</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parental Permission</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.ParentalPermissionAssent</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parental Permission Assent</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.ShortForm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Short Form</t>
   </si>
   <si>
+    <t xml:space="preserve">DeterminationApplication.Exempt</t>
+  </si>
+  <si>
     <t xml:space="preserve">Determination Application</t>
   </si>
   <si>
     <t xml:space="preserve">Exempt</t>
   </si>
   <si>
+    <t xml:space="preserve">DeterminationApplication.Non-Engaged</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non-Engaged</t>
   </si>
   <si>
+    <t xml:space="preserve">DeterminationApplication.Non-HSR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non-HSR</t>
   </si>
   <si>
+    <t xml:space="preserve">DeterminationApplication.UVAAgent</t>
+  </si>
+  <si>
     <t xml:space="preserve">UVA Agent</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.DrugFactSheet</t>
+  </si>
+  <si>
     <t xml:space="preserve">Drug Device Document</t>
   </si>
   <si>
     <t xml:space="preserve">Drug Fact Sheet</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.FDACommunication</t>
+  </si>
+  <si>
     <t xml:space="preserve">FDA Communication</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.FDAMarketingClearanceDocumentationMedicalDevice</t>
+  </si>
+  <si>
     <t xml:space="preserve">FDA Marketing Clearance Documentation Medical Device</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.InstructionsforUse</t>
+  </si>
+  <si>
     <t xml:space="preserve">Instructions for Use</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.InvestigationalDeviceInstructionsforUse.Clinician</t>
+  </si>
+  <si>
     <t xml:space="preserve">Investigational Device Instructions for Use</t>
   </si>
   <si>
     <t xml:space="preserve">Clinician</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.InvestigationalDeviceInstructionsforUse.PatientSubject</t>
+  </si>
+  <si>
     <t xml:space="preserve">Patient Subject</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.InvestigatorBrochure</t>
+  </si>
+  <si>
     <t xml:space="preserve">Investigator Brochure</t>
   </si>
   <si>
     <t xml:space="preserve">Investigators Brochure</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.InvestigatorBrochureAddendum</t>
+  </si>
+  <si>
     <t xml:space="preserve">Investigator Brochure Addendum</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.IVRSIWRSIXRSManual</t>
+  </si>
+  <si>
     <t xml:space="preserve">IVRS IWRS IXRS Manual</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.OtherIDSDocument</t>
+  </si>
+  <si>
     <t xml:space="preserve">Other IDS Document</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.PackageInsert</t>
+  </si>
+  <si>
     <t xml:space="preserve">Package Insert</t>
   </si>
   <si>
     <t xml:space="preserve">Package Inserts</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.PharmacistInstructionSheet</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pharmacist Instruction Sheet</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.PharmacyManual</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pharmacy Manual</t>
   </si>
   <si>
+    <t xml:space="preserve">DrugDeviceDocument.PrescriptionTemplate</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prescription Template</t>
   </si>
   <si>
+    <t xml:space="preserve">Form.DocumentSubmissionForm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Form</t>
   </si>
   <si>
     <t xml:space="preserve">Document Submission Form</t>
   </si>
   <si>
+    <t xml:space="preserve">Form.EmergencyUseNotification</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emergency Use Notification</t>
   </si>
   <si>
+    <t xml:space="preserve">Form.UnaffiliatedInvestigatorAgreementForm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unaffiliated Investigator Agreement Form</t>
   </si>
   <si>
+    <t xml:space="preserve">HIPAA.AuthorizationForm</t>
+  </si>
+  <si>
     <t xml:space="preserve">HIPAA</t>
   </si>
   <si>
     <t xml:space="preserve">Authorization Form</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-UVAIRB.ApprovalNewProtocolNon-UVAIRB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non-UVA IRB</t>
   </si>
   <si>
     <t xml:space="preserve">Approval New Protocol Non-UVA IRB</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-UVAIRB.IRBRelianceAgreement.Non-USAIRB</t>
+  </si>
+  <si>
     <t xml:space="preserve">IRB Reliance Agreement</t>
   </si>
   <si>
@@ -229,18 +370,33 @@
     <t xml:space="preserve">IRB Reliance Agreement Request Form- IRB-HSR Not IRB of Record</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-UVAIRB.IRBRelianceAgreement.USAIRB</t>
+  </si>
+  <si>
     <t xml:space="preserve">USA IRB</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-UVAIRB.LocalConsentLanguage</t>
+  </si>
+  <si>
     <t xml:space="preserve">Local Consent Language</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-UVAIRB.RelianceAgreementRequestForm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reliance Agreement Request Form</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-UVAIRB.StudyProtocolCoversheet</t>
+  </si>
+  <si>
     <t xml:space="preserve">Study Protocol Coversheet</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.Application.DepartmentChairSignature</t>
+  </si>
+  <si>
     <t xml:space="preserve">Study</t>
   </si>
   <si>
@@ -253,42 +409,75 @@
     <t xml:space="preserve">System</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.Application.InvestigatorAgreement</t>
+  </si>
+  <si>
     <t xml:space="preserve">Investigator Agreement</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.Application.PISignature</t>
+  </si>
+  <si>
     <t xml:space="preserve">PI Signature</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.Coversheet</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coversheet</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.DataSecurityPlan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Data Security Plan</t>
   </si>
   <si>
     <t xml:space="preserve">InfoSec Approval</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.Pre-ScreeningQuestions</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pre-Screening Questions</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.Protocol.Appendix</t>
+  </si>
+  <si>
     <t xml:space="preserve">Protocol</t>
   </si>
   <si>
     <t xml:space="preserve">Appendix</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.Protocol.Document</t>
+  </si>
+  <si>
     <t xml:space="preserve">Document</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.ProtocolSub-Study</t>
+  </si>
+  <si>
     <t xml:space="preserve">Protocol Sub-Study</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.ScreeningLog</t>
+  </si>
+  <si>
     <t xml:space="preserve">Screening Log</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.SurveyQuestionnaire</t>
+  </si>
+  <si>
     <t xml:space="preserve">Survey Questionnaire</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.ESCROApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">UVA Compliance</t>
   </si>
   <si>
@@ -298,69 +487,111 @@
     <t xml:space="preserve">Committee Member</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.GMEC</t>
+  </si>
+  <si>
     <t xml:space="preserve">GMEC</t>
   </si>
   <si>
     <t xml:space="preserve">GMEC Approval</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.GRIME</t>
+  </si>
+  <si>
     <t xml:space="preserve">GRIME</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.HIREApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">HIRE Approval</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.IBCApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">IBC Approval</t>
   </si>
   <si>
     <t xml:space="preserve">Institutional Biosafety Committee Approval</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.IDSNotification</t>
+  </si>
+  <si>
     <t xml:space="preserve">IDS Notification</t>
   </si>
   <si>
     <t xml:space="preserve">IDS - Investigational Drug Service Approval</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.IDSWaiverApplication</t>
+  </si>
+  <si>
     <t xml:space="preserve">IDS Waiver Application</t>
   </si>
   <si>
     <t xml:space="preserve">IDS Waiver</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.MRPhysicistApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">MR Physicist Approval</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.NewMedicalDeviceApplication</t>
+  </si>
+  <si>
     <t xml:space="preserve">New Medical Device Application</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.PRCApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">PRC Approval</t>
   </si>
   <si>
     <t xml:space="preserve">Cancer Center's PRC Approval Form</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.PRCWaiver</t>
+  </si>
+  <si>
     <t xml:space="preserve">PRC Waiver</t>
   </si>
   <si>
     <t xml:space="preserve">Cancer Center's PRC Approval waiver</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.RDRCApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">RDRC Approval</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.SBSFERPAApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">SBS FERPA Approval</t>
   </si>
   <si>
     <t xml:space="preserve">SBS/IRB Approval-FERPA</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.ScientificReviewApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">Scientific Review Approval</t>
   </si>
   <si>
     <t xml:space="preserve">Scientific Pre-review Documentation</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.SOMCTOApproval.IDEReviewLetter</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOM CTO Approval</t>
   </si>
   <si>
@@ -370,27 +601,45 @@
     <t xml:space="preserve">SOM CTO IND/IDE Review Letter</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.SOMCTOApproval.INDReviewLetter</t>
+  </si>
+  <si>
     <t xml:space="preserve">IND Review Letter</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.SOMCTOApproval.Non-UVAAcademiaPIofIDE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non-UVA Academia PI of IDE</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.SOMCTOApproval.Non-UVAAcademiaPIofIND</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non-UVA Academia PI of IND</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.SOMCTOApproval.Non-UVANon-IndustryPIofMultisiteStudy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non-UVA Non-Industry PI of Multisite Study</t>
   </si>
   <si>
     <t xml:space="preserve"> IRB Approval or Letter of Approval from Administration: Study Conducted at non- UVA Facilities</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.SOMCTOApproval.UVAPIMultisiteStudy</t>
+  </si>
+  <si>
     <t xml:space="preserve">UVA PI Multisite Study</t>
   </si>
   <si>
     <t xml:space="preserve">SOM CTO Approval Letter - UVA PI Multisite Trial</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.SOMCTOReview.RegardingNeedforIDE</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOM CTO Review</t>
   </si>
   <si>
@@ -400,34 +649,79 @@
     <t xml:space="preserve">SOM CTO Review regarding need for IDE</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.SOMCTOReview.RegardingNeedforIND</t>
+  </si>
+  <si>
     <t xml:space="preserve">Regarding Need for IND</t>
   </si>
   <si>
     <t xml:space="preserve">SOM CTO Review regarding need for IND</t>
   </si>
   <si>
+    <t xml:space="preserve">UVACompliance.SOMCTORevieworApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">SOM CTO Review or Approval</t>
   </si>
   <si>
+    <t xml:space="preserve">UVASIRB.RelianceAgreementRequestForm</t>
+  </si>
+  <si>
     <t xml:space="preserve">UVA SIRB</t>
   </si>
   <si>
+    <t xml:space="preserve">Study.Application.Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study.Application.DocumentwithSignatures</t>
+  </si>
+  <si>
     <t xml:space="preserve">Document with Signatures</t>
   </si>
   <si>
+    <t xml:space="preserve">UVASIRB.AssuranceForm.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Assurance Form</t>
   </si>
   <si>
+    <t xml:space="preserve">UVASIRB.CedingLetter</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ceding Letter</t>
   </si>
   <si>
+    <t xml:space="preserve">UVASIRB.IRBRelianceAgreement.Non-USAIRB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UVASIRB.IRBRelianceAgreement.USAIRB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AncillaryDocument.CoCApproval</t>
+  </si>
+  <si>
     <t xml:space="preserve">CoC Approval</t>
   </si>
   <si>
+    <t xml:space="preserve">Consent.Addendum.Prisoner</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prisoner</t>
   </si>
   <si>
+    <t xml:space="preserve">HIPAA.DataUseAgreement</t>
+  </si>
+  <si>
     <t xml:space="preserve">Data Use Agreement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-UVAIRB.Application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-UVAIRB.AssuranceForm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-UVAIRB.CedingLetter</t>
   </si>
 </sst>
 </file>
@@ -535,27 +829,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="B47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E64" activeCellId="0" sqref="E64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A98" activeCellId="0" sqref="A1:A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -573,1504 +868,1798 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>10</v>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>14</v>
+      <c r="G4" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>9</v>
+        <v>37</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>9</v>
+        <v>78</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>9</v>
+        <v>80</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F34" s="0" t="s">
-        <v>49</v>
+      <c r="G34" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="F38" s="0" t="s">
-        <v>54</v>
+      <c r="G38" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="F47" s="0" t="s">
-        <v>68</v>
+      <c r="G47" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="F48" s="0" t="s">
-        <v>68</v>
+      <c r="G48" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>8</v>
+        <v>119</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>8</v>
+        <v>123</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>76</v>
+        <v>127</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>76</v>
+        <v>130</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>76</v>
+        <v>132</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>8</v>
+        <v>136</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E56" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F56" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="F56" s="0" t="s">
-        <v>81</v>
+      <c r="G56" s="0" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>8</v>
+        <v>139</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>73</v>
+        <v>140</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>9</v>
+        <v>142</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>9</v>
+        <v>144</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>73</v>
+        <v>145</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>8</v>
+        <v>146</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>73</v>
+        <v>149</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>89</v>
+        <v>151</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E63" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F63" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="F63" s="0" t="s">
-        <v>90</v>
+      <c r="G63" s="0" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>8</v>
+        <v>156</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E64" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F64" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="F64" s="0" t="s">
-        <v>93</v>
+      <c r="G64" s="0" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>8</v>
+        <v>159</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>91</v>
+        <v>10</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>95</v>
+        <v>152</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>8</v>
+        <v>161</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E66" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F66" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="F66" s="0" t="s">
-        <v>95</v>
+      <c r="G66" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E67" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F67" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="F67" s="0" t="s">
-        <v>97</v>
+      <c r="G67" s="0" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="F68" s="0" t="s">
-        <v>99</v>
+      <c r="G68" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>89</v>
+        <v>168</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="F69" s="0" t="s">
-        <v>101</v>
+      <c r="G69" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>89</v>
+        <v>171</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>91</v>
+        <v>10</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>8</v>
+        <v>174</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>89</v>
+        <v>175</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="F72" s="0" t="s">
-        <v>105</v>
+      <c r="G72" s="0" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>89</v>
+        <v>178</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F73" s="0" t="s">
-        <v>107</v>
+        <v>10</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>89</v>
+        <v>181</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>108</v>
+        <v>152</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>8</v>
+        <v>182</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E74" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F74" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="F74" s="0" t="s">
-        <v>108</v>
+      <c r="G74" s="0" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>89</v>
+        <v>183</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E75" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F75" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="F75" s="0" t="s">
-        <v>110</v>
+      <c r="G75" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>89</v>
+        <v>186</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>111</v>
+        <v>152</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>8</v>
+        <v>187</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E76" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F76" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="F76" s="0" t="s">
-        <v>112</v>
+      <c r="G76" s="0" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>114</v>
+        <v>190</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E77" s="0" t="n">
+        <v>191</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F77" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F77" s="0" t="s">
-        <v>115</v>
+      <c r="G77" s="0" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>116</v>
+        <v>190</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E78" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F78" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F78" s="0" t="s">
-        <v>115</v>
+      <c r="G78" s="0" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>89</v>
+        <v>195</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>117</v>
+        <v>190</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>91</v>
+        <v>196</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>118</v>
+        <v>190</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>91</v>
+        <v>198</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>89</v>
+        <v>199</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>119</v>
+        <v>190</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E81" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F81" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="F81" s="0" t="s">
-        <v>120</v>
+      <c r="G81" s="0" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>89</v>
+        <v>202</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>121</v>
+        <v>190</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E82" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F82" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="F82" s="0" t="s">
-        <v>122</v>
+      <c r="G82" s="0" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>89</v>
+        <v>205</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>124</v>
+        <v>206</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="0" t="n">
+        <v>207</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="F83" s="0" t="s">
-        <v>125</v>
+      <c r="G83" s="0" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>89</v>
+        <v>209</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>126</v>
+        <v>206</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="F84" s="0" t="s">
-        <v>127</v>
+      <c r="G84" s="0" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>89</v>
+        <v>212</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>8</v>
+        <v>213</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>91</v>
+        <v>10</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>129</v>
+        <v>214</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>71</v>
+        <v>215</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>73</v>
+        <v>216</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>9</v>
+        <v>144</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>73</v>
+        <v>217</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>9</v>
+        <v>218</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>129</v>
+        <v>219</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="D89" s="0" t="s">
-        <v>9</v>
+        <v>215</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>129</v>
+        <v>221</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>132</v>
+        <v>215</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>8</v>
+        <v>222</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>129</v>
+        <v>223</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>66</v>
+        <v>215</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>9</v>
+        <v>114</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>129</v>
+        <v>224</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>66</v>
+        <v>215</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>9</v>
+        <v>117</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>6</v>
+        <v>225</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>8</v>
+        <v>226</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>11</v>
+        <v>227</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>134</v>
+        <v>34</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>9</v>
+        <v>228</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>62</v>
+        <v>229</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>8</v>
+        <v>230</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E95" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>64</v>
+        <v>231</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>8</v>
+        <v>126</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>64</v>
+        <v>232</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>8</v>
+        <v>220</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>64</v>
+        <v>233</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>8</v>
+        <v>222</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>